<commit_message>
klink modell, null steg tilbake
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Simple_extended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/28.03.2025/Simple_extended/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF78F4C9-4783-4987-9966-589890ED8FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{BF78F4C9-4783-4987-9966-589890ED8FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D98DC13D-DFA2-453D-B215-81AC77470D32}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="27" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="19" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -410,21 +410,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Info: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Retreived from GENeSYS-MOD data</t>
-    </r>
-  </si>
-  <si>
     <t>Info: Electric Boilers and Heat Pump size: https://ens.dk/sites/ens.dk/files/Analyser/technology_data_catalogue_for_industrial_process_heat.pdf. PV: https://coldwellsolar.com/commercial-solar-blog/what-kind-of-solar-array-is-needed-to-power-an-industrial-plant/ , P2G: https://en.wikipedia.org/wiki/Power-to-gas G2P: https://petrowiki.spe.org/Gas_to_power . For GasBoiler: https://www.linkedin.com/pulse/gas-fired-boilers-market-analysis-report-global-insights-region-7ccbc For CHP:  https://iea.blob.core.windows.net/assets/d459f7d5-1ba7-49d9-ad56-915fba22f267/chp_report.pdf</t>
   </si>
   <si>
@@ -581,6 +566,32 @@
   </si>
   <si>
     <t>HP_MT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Info: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Retreived from GENeSYS-MOD data</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Og regjeringen.no)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1100,7 +1111,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
@@ -1108,7 +1119,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1122,7 +1133,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1136,7 +1147,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1178,10 +1189,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1192,10 +1203,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1206,7 +1217,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -1220,7 +1231,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -1234,7 +1245,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -1248,7 +1259,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -1262,10 +1273,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1276,10 +1287,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1290,7 +1301,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1304,7 +1315,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -1318,7 +1329,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -1332,7 +1343,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -1346,7 +1357,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1360,7 +1371,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -1446,7 +1457,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1457,7 +1468,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>50</v>
@@ -1482,7 +1493,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1496,7 +1507,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -1510,7 +1521,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -1524,7 +1535,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -1580,7 +1591,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1594,7 +1605,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -1608,7 +1619,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -1622,7 +1633,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1636,7 +1647,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -1650,7 +1661,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -1664,7 +1675,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -1678,7 +1689,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1692,7 +1703,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -1706,7 +1717,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -1720,7 +1731,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -1734,7 +1745,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -1749,7 +1760,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -1763,7 +1774,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -1777,7 +1788,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -1791,7 +1802,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -1805,7 +1816,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1819,7 +1830,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -1861,10 +1872,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
         <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1898,12 +1909,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,7 +1935,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1932,7 +1943,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1940,7 +1951,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1972,7 +1983,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1980,7 +1991,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2005,7 +2016,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2055,7 +2066,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,7 +2202,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -2474,7 +2485,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -2491,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -2523,7 +2534,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2534,7 +2545,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2545,7 +2556,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2556,7 +2567,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2600,7 +2611,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2611,7 +2622,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2622,7 +2633,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2633,7 +2644,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2644,7 +2655,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -2655,7 +2666,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -2666,7 +2677,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2677,7 +2688,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2688,7 +2699,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -2699,7 +2710,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -2710,7 +2721,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -2721,7 +2732,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -2776,7 +2787,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2923,7 +2934,7 @@
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,7 +2947,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2944,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3002,7 +3013,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -3181,10 +3192,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C9CE7A-0F26-4BD5-B7D8-A3ADE3482E68}">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,7 +3208,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3206,14 +3217,6 @@
       </c>
       <c r="B4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3240,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3253,7 +3256,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3261,7 +3264,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3269,7 +3272,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3301,7 +3304,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3309,7 +3312,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3333,7 +3336,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3370,17 +3373,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -3400,12 +3403,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3420,7 +3423,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3456,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A3:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3468,10 +3471,10 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>52</v>
@@ -3531,7 +3534,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,12 +3544,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -3556,7 +3559,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>6.9400000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3567,27 +3570,22 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
-  <dimension ref="A3:A5"/>
+  <dimension ref="A3:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3619,12 +3617,12 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -3635,7 +3633,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -3646,7 +3644,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -3679,10 +3677,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3690,10 +3688,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -3701,7 +3699,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -3712,7 +3710,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -3723,7 +3721,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -3734,7 +3732,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -3745,10 +3743,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3756,10 +3754,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3767,7 +3765,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -3778,7 +3776,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -3789,7 +3787,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -3800,7 +3798,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -3811,7 +3809,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -3822,7 +3820,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -3894,7 +3892,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3910,7 +3908,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -3921,7 +3919,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -3932,7 +3930,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -3943,7 +3941,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -3987,7 +3985,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -3998,7 +3996,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -4010,7 +4008,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -4022,7 +4020,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -4033,7 +4031,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -4044,7 +4042,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -4055,7 +4053,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -4066,7 +4064,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -4077,7 +4075,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -4088,7 +4086,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -4099,7 +4097,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -4110,7 +4108,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -4121,7 +4119,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -4132,7 +4130,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -4143,7 +4141,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -4154,7 +4152,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -4165,7 +4163,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -4176,7 +4174,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -4209,10 +4207,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
         <v>87</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -4277,7 +4275,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4415,7 +4413,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4428,7 +4426,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>100000</v>
@@ -4436,7 +4434,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>100000</v>
@@ -4444,7 +4442,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>100000</v>
@@ -4476,7 +4474,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -4484,7 +4482,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>100000</v>
@@ -4508,7 +4506,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>100000</v>
@@ -4537,7 +4535,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4616,7 +4614,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4633,7 +4631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -4644,7 +4642,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4662,7 +4660,7 @@
   <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4674,10 +4672,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4698,7 +4696,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>20.8</v>
@@ -4706,7 +4704,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>119.2</v>
@@ -4714,7 +4712,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>143.80000000000001</v>
@@ -4746,7 +4744,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -4754,7 +4752,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>274</v>
@@ -4778,7 +4776,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4823,7 +4821,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4951,7 +4949,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -4986,12 +4984,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4999,7 +4997,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5084,7 +5082,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5254,14 +5252,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5466,27 +5462,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5511,9 +5500,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
sett/data for loadshift fikset
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/28.03.2025/Simple_extended/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\simple_extended_v2\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{BF78F4C9-4783-4987-9966-589890ED8FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D98DC13D-DFA2-453D-B215-81AC77470D32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EE5FA-DF65-453A-87DD-68E702407913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="19" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="20" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -41,8 +41,8 @@
     <sheet name="Set_of_PeriodsInMonth" sheetId="73" r:id="rId26"/>
     <sheet name="Par_Ramping_factor" sheetId="64" r:id="rId27"/>
     <sheet name="Set_of_Technology" sheetId="35" r:id="rId28"/>
-    <sheet name="Subset_LoadShiftWindow" sheetId="37" r:id="rId29"/>
-    <sheet name="Set_of_LoadShiftingInterval" sheetId="46" r:id="rId30"/>
+    <sheet name="Set_of_TimeSteps_NO_LoadShift" sheetId="37" r:id="rId29"/>
+    <sheet name="Set_of_LoadShiftingPeriod" sheetId="46" r:id="rId30"/>
     <sheet name="Subset_ECToTech" sheetId="40" r:id="rId31"/>
     <sheet name="Subset_TechToEC" sheetId="41" r:id="rId32"/>
     <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId33"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="96">
   <si>
     <t>Benevning:</t>
   </si>
@@ -357,9 +357,6 @@
   </si>
   <si>
     <t>Month</t>
-  </si>
-  <si>
-    <t>TimeLoadShift</t>
   </si>
   <si>
     <t>Unit: Fraction</t>
@@ -456,9 +453,6 @@
   </si>
   <si>
     <t>Energy2Power</t>
-  </si>
-  <si>
-    <t>Intervals</t>
   </si>
   <si>
     <r>
@@ -592,6 +586,9 @@
       </rPr>
       <t xml:space="preserve"> Og regjeringen.no)</t>
     </r>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1092,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,7 +1108,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
@@ -1119,7 +1116,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1133,7 +1130,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1147,7 +1144,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1189,10 +1186,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1203,10 +1200,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1217,7 +1214,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -1231,7 +1228,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -1245,7 +1242,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -1273,10 +1270,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1287,10 +1284,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1301,7 +1298,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -1329,7 +1326,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -1343,7 +1340,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -1357,7 +1354,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1371,7 +1368,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -1452,12 +1449,12 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1468,7 +1465,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>50</v>
@@ -1493,7 +1490,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1507,7 +1504,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -1521,7 +1518,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -1535,7 +1532,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1605,7 +1602,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -1619,7 +1616,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -1633,7 +1630,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1647,7 +1644,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -1661,7 +1658,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -1675,7 +1672,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -1689,7 +1686,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1703,7 +1700,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -1731,7 +1728,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -1745,7 +1742,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -1760,7 +1757,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -1774,7 +1771,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -1788,7 +1785,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -1802,7 +1799,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -1816,7 +1813,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1830,7 +1827,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -1872,10 +1869,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1909,12 +1906,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1935,7 +1932,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1943,7 +1940,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1951,7 +1948,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1983,7 +1980,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1991,7 +1988,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2016,7 +2013,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2066,12 +2063,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2189,12 +2186,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,7 +2199,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -2284,12 +2281,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,7 +2379,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2443,12 +2440,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2485,7 +2482,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -2502,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -2534,7 +2531,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2545,7 +2542,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2556,7 +2553,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2567,7 +2564,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2611,7 +2608,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2622,7 +2619,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2633,7 +2630,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2644,7 +2641,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2655,7 +2652,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -2666,7 +2663,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -2677,7 +2674,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2699,7 +2696,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -2710,7 +2707,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -2732,7 +2729,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -2787,7 +2784,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2934,7 +2931,7 @@
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,7 +2944,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2955,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3013,7 +3010,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -3192,10 +3189,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C9CE7A-0F26-4BD5-B7D8-A3ADE3482E68}">
-  <dimension ref="A3:B4"/>
+  <dimension ref="A3:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,7 +3205,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3217,6 +3214,14 @@
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3243,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3256,7 +3261,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3264,7 +3269,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3272,7 +3277,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3304,7 +3309,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3312,7 +3317,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3336,7 +3341,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3373,17 +3378,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -3403,12 +3408,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3423,7 +3428,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3457,71 +3462,247 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A3:C7"/>
+  <dimension ref="A3:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="B6">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="B19">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="B7">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>3</v>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3544,12 +3725,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -3572,20 +3753,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3617,12 +3798,12 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -3633,7 +3814,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -3644,7 +3825,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -3677,10 +3858,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3688,10 +3869,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -3699,7 +3880,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -3710,7 +3891,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -3721,7 +3902,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -3732,7 +3913,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -3743,10 +3924,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3754,10 +3935,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3765,7 +3946,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -3776,7 +3957,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -3787,7 +3968,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -3798,7 +3979,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -3809,7 +3990,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -3820,7 +4001,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -3892,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3908,7 +4089,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -3919,7 +4100,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -3930,7 +4111,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -3941,7 +4122,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -3985,7 +4166,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -3996,7 +4177,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -4008,7 +4189,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -4020,7 +4201,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -4031,7 +4212,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -4042,7 +4223,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -4053,7 +4234,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -4064,7 +4245,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -4075,7 +4256,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -4086,7 +4267,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -4097,7 +4278,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -4108,7 +4289,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -4119,7 +4300,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -4130,7 +4311,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -4141,7 +4322,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -4152,7 +4333,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -4163,7 +4344,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -4174,7 +4355,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -4207,10 +4388,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -4275,7 +4456,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4413,7 +4594,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4426,7 +4607,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>100000</v>
@@ -4434,7 +4615,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>100000</v>
@@ -4442,7 +4623,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>100000</v>
@@ -4474,7 +4655,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -4482,7 +4663,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>100000</v>
@@ -4506,7 +4687,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>100000</v>
@@ -4535,7 +4716,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4614,7 +4795,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4642,7 +4823,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4672,10 +4853,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4696,7 +4877,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>20.8</v>
@@ -4704,7 +4885,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6">
         <v>119.2</v>
@@ -4712,7 +4893,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>143.80000000000001</v>
@@ -4744,7 +4925,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -4752,7 +4933,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>274</v>
@@ -4776,7 +4957,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4821,7 +5002,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4949,7 +5130,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -4984,12 +5165,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4997,7 +5178,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5082,7 +5263,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5252,12 +5433,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5462,20 +5645,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5500,18 +5690,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
oppdatert data for self-discharge
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\simple_extended_v2\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EE5FA-DF65-453A-87DD-68E702407913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659E9DFD-A0F8-4FAE-8AFA-129BD1DF4C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="20" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -2833,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,8 +2866,8 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f>0.1/24</f>
-        <v>4.1666666666666666E-3</v>
+        <f>0.001/24</f>
+        <v>4.1666666666666665E-5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,8 +2900,8 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <f>0.2/24</f>
-        <v>8.3333333333333332E-3</v>
+        <f>0.002/24</f>
+        <v>8.3333333333333331E-5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2931,7 +2931,7 @@
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3189,10 +3189,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C9CE7A-0F26-4BD5-B7D8-A3ADE3482E68}">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,14 +3214,6 @@
       </c>
       <c r="B4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3462,10 +3454,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A3:B31"/>
+  <dimension ref="A3:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,118 +3583,6 @@
       </c>
       <c r="B17">
         <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>7</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>8</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>21</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>22</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>23</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>24</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3753,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,7 +3646,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4841,7 +4721,7 @@
   <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4880,7 +4760,7 @@
         <v>75</v>
       </c>
       <c r="B5">
-        <v>20.8</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4888,7 +4768,7 @@
         <v>92</v>
       </c>
       <c r="B6">
-        <v>119.2</v>
+        <v>166.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4896,7 +4776,7 @@
         <v>93</v>
       </c>
       <c r="B7">
-        <v>143.80000000000001</v>
+        <v>199.6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4904,7 +4784,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>62.6</v>
+        <v>105.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4912,7 +4792,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>82.1</v>
+        <v>137.44999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4920,7 +4800,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>378.1</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4928,7 +4808,7 @@
         <v>76</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4936,7 +4816,7 @@
         <v>77</v>
       </c>
       <c r="B12">
-        <v>274</v>
+        <v>174.5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4991,7 +4871,7 @@
   <dimension ref="A2:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5018,7 +4898,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>152.05000000000001</v>
+        <v>178.36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5026,7 +4906,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>87.7</v>
+        <v>101.8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5034,7 +4914,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>47.3</v>
+        <v>121.4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5042,7 +4922,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>21.1</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5050,7 +4930,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5058,7 +4938,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>6.7</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5066,7 +4946,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>0.03</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5433,14 +5313,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5645,27 +5523,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5690,9 +5561,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
La til kostnad load shift
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4dbc8342d6ca6595/Documents/INDØK 10. semester/Master_multi-stage/Simple_extended-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v5\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{659E9DFD-A0F8-4FAE-8AFA-129BD1DF4C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A55CE9BC-7E78-4199-885E-B6D7B2000B30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC1909-26F6-41E7-9D10-FDE6E87EE558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="1000" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="21" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -42,10 +42,11 @@
     <sheet name="Subset_TechToEC" sheetId="41" r:id="rId27"/>
     <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId28"/>
     <sheet name="Par_BatteryCost" sheetId="55" r:id="rId29"/>
-    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId30"/>
-    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId31"/>
-    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId32"/>
-    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId33"/>
+    <sheet name="Par_Cost_LS" sheetId="74" r:id="rId30"/>
+    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId31"/>
+    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId32"/>
+    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId33"/>
+    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="92">
   <si>
     <t>Benevning:</t>
   </si>
@@ -522,6 +523,9 @@
   </si>
   <si>
     <t>H2_Grid</t>
+  </si>
+  <si>
+    <t>CostLS</t>
   </si>
 </sst>
 </file>
@@ -974,27 +978,27 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -1012,23 +1016,23 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1042,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1104,28 +1108,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1138,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1203,24 +1207,24 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1229,7 +1233,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1237,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1253,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1277,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1298,27 +1302,27 @@
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -1336,17 +1340,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -1364,27 +1368,27 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>130000</v>
       </c>
@@ -1402,23 +1406,23 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1435,7 +1439,7 @@
         <v>4.1666666666666665E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1443,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1451,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1473,7 @@
         <v>8.3333333333333331E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>4.1666666666666669E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1499,52 +1503,52 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
   </sheetData>
@@ -1560,47 +1564,47 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1618,13 +1622,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1664,7 +1668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1701,22 +1705,22 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1728,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1737,7 +1741,7 @@
       <c r="D3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1759,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1836,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1847,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1858,7 +1862,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1913,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -1935,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -1946,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -2001,7 +2005,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2012,7 +2016,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2023,7 +2027,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2045,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -2078,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2089,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -2100,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -2111,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -2144,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -2155,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>71</v>
       </c>
@@ -2166,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>82</v>
       </c>
@@ -2177,7 +2181,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>90</v>
       </c>
@@ -2188,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>90</v>
       </c>
@@ -2199,25 +2203,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -2234,14 +2238,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2259,12 +2263,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
@@ -2272,7 +2276,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2280,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2309,13 +2313,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2347,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2355,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2363,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -2403,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2427,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2435,7 +2439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -2464,118 +2468,118 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="D25" s="4"/>
     </row>
@@ -2592,12 +2596,12 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
@@ -2605,7 +2609,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2613,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2621,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2637,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2645,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2653,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2661,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2669,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2685,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -2693,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>22</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24</v>
       </c>
@@ -2717,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2733,7 +2737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2741,7 +2745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2749,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2757,7 +2761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2765,7 +2769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2781,7 +2785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2797,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>21</v>
       </c>
@@ -2805,7 +2809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>22</v>
       </c>
@@ -2813,7 +2817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>23</v>
       </c>
@@ -2821,7 +2825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>24</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2845,7 +2849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2861,7 +2865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2869,7 +2873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -2885,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2893,7 +2897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -2901,7 +2905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -2909,7 +2913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>21</v>
       </c>
@@ -2917,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>22</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>23</v>
       </c>
@@ -2933,7 +2937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>24</v>
       </c>
@@ -2954,19 +2958,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2984,15 +2988,15 @@
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3003,7 +3007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3014,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -3025,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -3036,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -3047,7 +3051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3058,7 +3062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3069,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -3080,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -3091,7 +3095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -3102,7 +3106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -3113,7 +3117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3124,7 +3128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -3135,7 +3139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -3146,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -3157,7 +3161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -3179,7 +3183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -3201,7 +3205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3212,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3223,7 +3227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3234,7 +3238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3245,7 +3249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3256,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -3267,7 +3271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -3289,7 +3293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3300,7 +3304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -3322,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -3355,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
@@ -3366,7 +3370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -3377,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -3388,7 +3392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>90</v>
       </c>
@@ -3414,14 +3418,14 @@
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3432,7 +3436,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3443,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3465,7 +3469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -3476,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -3487,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -3498,7 +3502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3509,7 +3513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3520,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -3531,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3554,7 +3558,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -3566,7 +3570,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3577,7 +3581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -3588,7 +3592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -3599,7 +3603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -3610,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -3621,7 +3625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -3632,7 +3636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -3643,7 +3647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -3654,7 +3658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -3665,7 +3669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3676,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3687,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -3698,7 +3702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -3709,7 +3713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -3720,7 +3724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -3753,7 +3757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -3764,7 +3768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3775,7 +3779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -3797,7 +3801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -3808,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -3819,7 +3823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3830,7 +3834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -3841,7 +3845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -3852,7 +3856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -3863,7 +3867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -3874,7 +3878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3885,7 +3889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -3896,7 +3900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -3907,7 +3911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -3918,7 +3922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -3929,7 +3933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -3940,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -3951,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -3962,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -3973,7 +3977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>90</v>
       </c>
@@ -3984,42 +3988,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="G65" s="4"/>
     </row>
@@ -4036,42 +4040,42 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4089,17 +4093,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4107,7 +4111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4115,7 +4119,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4123,7 +4127,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4131,7 +4135,7 @@
         <v>2.6160000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4139,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4147,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4155,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4176,27 +4180,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6.9400000000000003E-2</v>
       </c>
@@ -4208,6 +4212,88 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
+  <dimension ref="A3:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
   <dimension ref="A3:B19"/>
   <sheetViews>
@@ -4215,12 +4301,12 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4228,7 +4314,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4236,7 +4322,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -4244,7 +4330,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -4252,7 +4338,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -4260,7 +4346,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -4268,7 +4354,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -4276,7 +4362,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4284,7 +4370,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -4292,7 +4378,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -4300,7 +4386,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -4308,7 +4394,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4316,7 +4402,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -4324,7 +4410,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -4332,7 +4418,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -4340,7 +4426,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -4348,7 +4434,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -4361,7 +4447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -4369,12 +4455,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4382,7 +4468,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4390,7 +4476,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4398,7 +4484,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4406,7 +4492,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4414,7 +4500,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4422,7 +4508,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4430,7 +4516,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4443,7 +4529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB31CFC9-E7A6-4B4A-99A3-E708E722ECEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -4451,17 +4537,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100000000</v>
       </c>
@@ -4471,7 +4557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -4479,17 +4565,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000000</v>
       </c>
@@ -4507,23 +4593,23 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -4531,7 +4617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4539,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4548,7 +4634,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4557,7 +4643,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4565,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4574,7 +4660,7 @@
         <v>1.657142857142857E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4583,7 +4669,7 @@
         <v>5.9880239520958087E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4604,23 +4690,23 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4628,7 +4714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4637,7 +4723,7 @@
         <v>1.0204081632653061</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4645,7 +4731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4654,7 +4740,7 @@
         <v>1.1904761904761905</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4663,7 +4749,7 @@
         <v>1.0101010101010102</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4671,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4680,7 +4766,7 @@
         <v>1.1363636363636365</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4701,23 +4787,23 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -4725,7 +4811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4733,7 +4819,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4741,7 +4827,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4749,7 +4835,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -4757,7 +4843,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4765,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4773,7 +4859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4794,27 +4880,27 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4828,7 +4914,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -4842,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -4856,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -4870,7 +4956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -4884,7 +4970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4898,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4912,7 +4998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -4926,7 +5012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -4940,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4954,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -4968,7 +5054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -4982,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -4996,7 +5082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -5010,7 +5096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5024,7 +5110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -5038,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -5052,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -5066,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5080,7 +5166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -5094,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -5108,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -5122,7 +5208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -5136,7 +5222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -5150,7 +5236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -5164,7 +5250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -5178,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -5192,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5206,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -5220,7 +5306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -5234,7 +5320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -5248,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -5262,7 +5348,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -5276,7 +5362,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
@@ -5290,7 +5376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -5304,7 +5390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -5318,7 +5404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -5345,26 +5431,26 @@
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5378,7 +5464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5395,7 +5481,7 @@
       <c r="Q4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -5409,7 +5495,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -5423,7 +5509,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -5437,7 +5523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5451,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -5465,7 +5551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -5479,7 +5565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5493,7 +5579,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -5507,7 +5593,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -5521,7 +5607,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -5535,7 +5621,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -5549,7 +5635,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -5563,7 +5649,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -5577,7 +5663,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5591,7 +5677,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -5605,7 +5691,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -5619,7 +5705,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -5633,7 +5719,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -5647,7 +5733,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -5661,7 +5747,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -5675,7 +5761,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -5689,7 +5775,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -5703,7 +5789,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -5717,7 +5803,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -5731,7 +5817,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -5745,7 +5831,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -5760,7 +5846,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -5774,7 +5860,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -5788,7 +5874,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -5802,7 +5888,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -5816,7 +5902,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -5830,7 +5916,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -5844,7 +5930,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -5858,7 +5944,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -5872,7 +5958,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -5886,7 +5972,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -5900,7 +5986,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -5914,7 +6000,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -5928,7 +6014,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -5942,7 +6028,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -5956,7 +6042,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -5970,7 +6056,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -5984,7 +6070,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -5998,7 +6084,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -6012,7 +6098,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -6026,7 +6112,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -6040,7 +6126,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>71</v>
       </c>
@@ -6054,7 +6140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>82</v>
       </c>
@@ -6068,7 +6154,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -6095,24 +6181,24 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -6120,7 +6206,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6128,7 +6214,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -6136,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -6144,7 +6230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -6152,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6160,7 +6246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -6168,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -6176,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -6184,7 +6270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -6192,7 +6278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -6201,7 +6287,7 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -6210,7 +6296,7 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -6218,7 +6304,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -6226,7 +6312,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -6234,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>82</v>
       </c>
@@ -6243,7 +6329,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -6251,24 +6337,24 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
   </sheetData>
@@ -6478,6 +6564,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6486,15 +6581,6 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6517,6 +6603,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6531,12 +6625,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Endra kostnad gasskjel CCS
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v5\Simple_extended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v6\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC1909-26F6-41E7-9D10-FDE6E87EE558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C54E9F-BFD4-4464-9EDC-A6A79E8442E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="21" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -1701,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,7 +2123,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4215,7 +4215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
   <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -6363,6 +6363,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6563,27 +6583,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6600,29 +6625,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fiksa load shift i henhold til latex
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v6\Simple_extended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\V7\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C54E9F-BFD4-4464-9EDC-A6A79E8442E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCC73E4-97FC-42CB-89A0-AEBD2F58031B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="14" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="92">
   <si>
     <t>Benevning:</t>
   </si>
@@ -1296,35 +1296,226 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1334,25 +1525,216 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A3:A4"/>
+  <dimension ref="A3:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +2083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -2592,7 +2974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A3:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2954,7 +3336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -6363,26 +6745,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6583,32 +6945,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6625,4 +6982,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Max_Capex (endra til små bokstaver for solstorm)
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v8\Simple_extended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v1\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D22DF91-F9BD-44DB-99A8-BE65E6CD5EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="23" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="23" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -3361,7 +3361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
@@ -4938,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -6740,6 +6740,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6940,27 +6960,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6977,29 +7002,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Wide case instance 1 year 2025 klar for solstorm
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/25.04/Simple_extended-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DBFFC58-FF4C-4FD1-AE79-E1CA8CC38E03}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67742E50-1425-4703-889C-B3C83900FC1D}"/>
   <bookViews>
-    <workbookView xWindow="-390" yWindow="15" windowWidth="14790" windowHeight="15525" tabRatio="1000" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -46,16 +46,15 @@
     <sheet name="Par_Ramping_factor" sheetId="64" r:id="rId31"/>
     <sheet name="Set_of_Technology" sheetId="35" r:id="rId32"/>
     <sheet name="Set_of_TimeSteps_NO_LoadShift" sheetId="37" r:id="rId33"/>
-    <sheet name="Set_of_LoadShiftingPeriod" sheetId="46" r:id="rId34"/>
-    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId35"/>
-    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId36"/>
-    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId37"/>
-    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId38"/>
-    <sheet name="Par_Cost_LS" sheetId="74" r:id="rId39"/>
-    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId40"/>
-    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId41"/>
-    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId42"/>
-    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId43"/>
+    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId34"/>
+    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId35"/>
+    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId36"/>
+    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId37"/>
+    <sheet name="Par_Cost_LS" sheetId="74" r:id="rId38"/>
+    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId39"/>
+    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId40"/>
+    <sheet name="Par_Max_CAPEX" sheetId="69" r:id="rId41"/>
+    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="92">
   <si>
     <t>Benevning:</t>
   </si>
@@ -1109,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4745B9-33CD-4F54-B24F-2FB1EF9BEFBD}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +2921,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,7 +2955,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,7 +2963,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2972,7 +2971,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,7 +2979,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2988,7 +2987,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,7 +2995,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3003,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -3646,7 +3645,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,7 +3740,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5281,31 +5280,6 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
-  <dimension ref="A3:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:C39"/>
   <sheetViews>
@@ -5735,7 +5709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A3:I65"/>
   <sheetViews>
@@ -6357,7 +6331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
   <dimension ref="A3:A9"/>
   <sheetViews>
@@ -6410,7 +6384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815BD0D-D4C8-43C3-B5E1-419A131BCC6A}">
   <dimension ref="A2:B10"/>
   <sheetViews>
@@ -6497,7 +6471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -6572,6 +6546,160 @@
       </c>
       <c r="B10">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
+  <dimension ref="A3:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -6615,160 +6743,6 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
-  <dimension ref="A3:B19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19">
-        <v>100000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -6850,7 +6824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB31CFC9-E7A6-4B4A-99A3-E708E722ECEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -6878,7 +6852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -7082,6 +7056,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -7090,15 +7073,6 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7303,6 +7277,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -7315,14 +7297,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Må fortsatt endre mer ift. test input data med lagt til HT og Firect Firing til teknologier, men startet. Cost må også fikses før kjøring
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/25.04/Simple_extended-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/New folder/Simple_extended/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67742E50-1425-4703-889C-B3C83900FC1D}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC93E80-BE36-477C-A9BB-C759EBB945AF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="95">
   <si>
     <t>Benevning:</t>
   </si>
@@ -534,6 +534,15 @@
   </si>
   <si>
     <t>CostLS</t>
+  </si>
+  <si>
+    <t>Direct Firing</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>Direct_Firing</t>
   </si>
 </sst>
 </file>
@@ -707,10 +716,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1430,7 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -1981,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,7 +3021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -4794,7 +4799,7 @@
   <dimension ref="A3:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,7 +4894,9 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5281,10 +5288,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
-  <dimension ref="A3:C39"/>
+  <dimension ref="A3:C52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5406,7 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -5421,7 +5428,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -5432,7 +5439,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -5440,35 +5447,35 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5476,10 +5483,10 @@
         <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5487,10 +5494,10 @@
         <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5498,81 +5505,81 @@
         <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -5583,7 +5590,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -5594,10 +5601,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -5605,7 +5612,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -5616,10 +5623,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -5627,79 +5634,222 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>71</v>
+      <c r="A34" t="s">
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>71</v>
+      <c r="A35" t="s">
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>2</v>
+      <c r="A36" t="s">
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B51" t="s">
         <v>30</v>
       </c>
-      <c r="C39">
+      <c r="C51">
         <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5711,10 +5861,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A3:I65"/>
+  <dimension ref="A3:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,7 +6012,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -5874,7 +6024,7 @@
         <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -5885,7 +6035,7 @@
         <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -5896,7 +6046,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -5904,35 +6054,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5940,10 +6090,10 @@
         <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5951,10 +6101,10 @@
         <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5962,54 +6112,54 @@
         <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6020,7 +6170,7 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6031,7 +6181,7 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6042,7 +6192,7 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6053,7 +6203,7 @@
         <v>29</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6061,10 +6211,10 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6075,7 +6225,7 @@
         <v>29</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6083,10 +6233,10 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6097,117 +6247,117 @@
         <v>29</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6215,10 +6365,10 @@
         <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6229,102 +6379,256 @@
         <v>29</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="G60" s="4"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63">
+        <v>9</v>
+      </c>
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64">
+        <v>9</v>
+      </c>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="G65" s="4"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B69" t="s">
         <v>30</v>
       </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="G60" s="4"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="G61" s="4"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="G63" s="4"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="G64" s="4"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="G65" s="4"/>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6333,10 +6637,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
-  <dimension ref="A3:A9"/>
+  <dimension ref="A3:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6377,6 +6681,21 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6473,10 +6792,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
-  <dimension ref="A3:B10"/>
+  <dimension ref="A3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6518,15 +6837,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6534,7 +6853,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6542,9 +6861,17 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
@@ -6555,10 +6882,10 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
-  <dimension ref="A3:B19"/>
+  <dimension ref="A3:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6699,6 +7026,14 @@
         <v>90</v>
       </c>
       <c r="B19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20">
         <v>100000</v>
       </c>
     </row>
@@ -7056,26 +7391,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -7276,10 +7591,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7302,20 +7648,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Deep_case_test med ferdig input data
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61400315-CB3A-44F7-8E79-B455BEA47CF8}"/>
+  <xr:revisionPtr revIDLastSave="413" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05219CC9-55C2-43CF-99B4-2574697C1988}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="21" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="92">
   <si>
     <t>Benevning:</t>
   </si>
@@ -526,9 +526,6 @@
   </si>
   <si>
     <t>CostLS</t>
-  </si>
-  <si>
-    <t>Direct Firing</t>
   </si>
   <si>
     <t>HT</t>
@@ -1428,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2137,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
@@ -2154,7 +2151,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
@@ -2168,7 +2165,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
         <v>31</v>
@@ -2191,7 +2188,7 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="A72" sqref="A72:A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2399,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2444,7 +2441,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -2486,7 +2483,7 @@
         <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -2528,7 +2525,7 @@
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2570,7 +2567,7 @@
         <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -2612,7 +2609,7 @@
         <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -2683,7 +2680,7 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2767,7 +2764,7 @@
         <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -2852,7 +2849,7 @@
         <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47">
         <v>9</v>
@@ -2940,7 +2937,7 @@
         <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -3026,7 +3023,7 @@
         <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -3110,7 +3107,7 @@
         <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -3205,7 +3202,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
         <v>34</v>
@@ -3219,7 +3216,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
         <v>35</v>
@@ -3233,10 +3230,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
         <v>90</v>
-      </c>
-      <c r="B74" t="s">
-        <v>91</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -3416,7 +3413,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3545,7 +3542,7 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="A58" sqref="A58:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4184,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4198,7 +4195,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -4209,7 +4206,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -5035,7 +5032,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -5420,7 +5417,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5435,8 +5432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A3:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5532,7 +5529,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -5566,7 +5563,7 @@
   <dimension ref="A3:C54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6118,7 +6115,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
@@ -6129,7 +6126,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
@@ -6140,7 +6137,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
         <v>31</v>
@@ -6160,7 +6157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A3:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:C74"/>
     </sheetView>
   </sheetViews>
@@ -6308,7 +6305,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -6341,7 +6338,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -6374,7 +6371,7 @@
         <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -6407,7 +6404,7 @@
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -6440,7 +6437,7 @@
         <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -6473,7 +6470,7 @@
         <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -6528,7 +6525,7 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -6594,7 +6591,7 @@
         <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -6660,7 +6657,7 @@
         <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47">
         <v>9</v>
@@ -6726,7 +6723,7 @@
         <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -6792,7 +6789,7 @@
         <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -6858,7 +6855,7 @@
         <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -6934,7 +6931,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
         <v>34</v>
@@ -6946,7 +6943,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
         <v>35</v>
@@ -6958,10 +6955,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -7175,7 +7172,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -7369,7 +7366,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20">
         <v>100000</v>
@@ -7495,7 +7492,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7729,6 +7726,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -7929,27 +7946,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7966,29 +7988,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
FIkset alt utenom kostnader fra Lasse før klink modell
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="413" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05219CC9-55C2-43CF-99B4-2574697C1988}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B583B9-8B57-41EA-8B0C-E0361A2C9B4C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="90">
   <si>
     <t>Benevning:</t>
   </si>
@@ -526,12 +526,6 @@
   </si>
   <si>
     <t>CostLS</t>
-  </si>
-  <si>
-    <t>HT</t>
-  </si>
-  <si>
-    <t>Direct_Firing</t>
   </si>
 </sst>
 </file>
@@ -702,10 +696,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1236,7 +1226,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:A54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1570,7 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1608,7 +1598,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -1622,7 +1612,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -1633,13 +1623,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1647,13 +1637,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1661,13 +1651,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1678,10 +1668,10 @@
         <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1692,10 +1682,10 @@
         <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1706,10 +1696,10 @@
         <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1717,13 +1707,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1731,13 +1721,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1745,13 +1735,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1759,13 +1749,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1773,13 +1763,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1787,13 +1777,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1801,7 +1791,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -1815,7 +1805,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -1829,10 +1819,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1843,7 +1833,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -1857,10 +1847,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -1871,10 +1861,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -1884,42 +1874,42 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>66</v>
+      <c r="A34" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>66</v>
+      <c r="A35" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>66</v>
+      <c r="A36" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1927,13 +1917,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1941,10 +1931,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1955,227 +1945,38 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42">
-        <v>6</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45">
-        <v>9</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>0.2</v>
-      </c>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>0.8</v>
-      </c>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
+      <c r="A48" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2187,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:A74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,7 +2200,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2413,7 +2214,7 @@
         <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2427,7 +2228,7 @@
         <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -2441,7 +2242,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -2452,13 +2253,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0.93</v>
@@ -2466,13 +2267,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>0.93</v>
@@ -2480,13 +2281,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D21">
         <v>0.93</v>
@@ -2497,10 +2298,10 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>0.93</v>
@@ -2511,10 +2312,10 @@
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>0.93</v>
@@ -2525,10 +2326,10 @@
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D24">
         <v>0.93</v>
@@ -2536,86 +2337,86 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.93</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0.93</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>0.93</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>0.93</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>0.93</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="C30">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>0.93</v>
+        <v>0.3</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -2624,10 +2425,10 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D31">
         <v>0.45</v>
@@ -2641,7 +2442,7 @@
         <v>29</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D32">
         <v>0.3</v>
@@ -2652,10 +2453,10 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>0.45</v>
@@ -2669,7 +2470,7 @@
         <v>29</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>0.3</v>
@@ -2680,10 +2481,10 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>0.45</v>
@@ -2697,7 +2498,7 @@
         <v>29</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>0.3</v>
@@ -2705,13 +2506,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>0.45</v>
@@ -2719,13 +2520,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>0.3</v>
@@ -2733,13 +2534,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <v>0.45</v>
@@ -2747,13 +2548,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D40">
         <v>0.3</v>
@@ -2761,13 +2562,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D41">
         <v>0.45</v>
@@ -2775,13 +2576,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D42">
         <v>0.3</v>
@@ -2789,13 +2590,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
         <v>0.45</v>
@@ -2803,13 +2604,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D44">
         <v>0.3</v>
@@ -2817,13 +2618,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>0.45</v>
@@ -2831,13 +2632,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>0.3</v>
@@ -2846,13 +2647,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D47">
         <v>0.45</v>
@@ -2861,13 +2662,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
         <v>29</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D48">
         <v>0.3</v>
@@ -2876,371 +2677,94 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>0.45</v>
+        <v>0.99990000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>0.3</v>
+        <v>0.99990000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>82</v>
+      <c r="A51" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>82</v>
+      <c r="A52" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>0.45</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="D54">
-        <v>0.3</v>
-      </c>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
-      </c>
-      <c r="D55">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
-      </c>
-      <c r="D56">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-      <c r="D57">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
-      <c r="D58">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-      <c r="D59">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60">
-        <v>6</v>
-      </c>
-      <c r="D60">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61">
-        <v>7</v>
-      </c>
-      <c r="D61">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C62">
-        <v>7</v>
-      </c>
-      <c r="D62">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63">
-        <v>8</v>
-      </c>
-      <c r="D63">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64">
-        <v>8</v>
-      </c>
-      <c r="D64">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65">
-        <v>9</v>
-      </c>
-      <c r="D65">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66">
-        <v>9</v>
-      </c>
-      <c r="D66">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B72" t="s">
-        <v>34</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" t="s">
-        <v>90</v>
-      </c>
-      <c r="C74">
-        <v>3</v>
-      </c>
-      <c r="D74">
-        <v>0.92</v>
-      </c>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3252,7 +2776,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3412,12 +2936,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -3541,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A60"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,7 +3240,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>160</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3743,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3754,40 +3273,40 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3795,7 +3314,7 @@
         <v>83</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3806,7 +3325,7 @@
         <v>83</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3817,7 +3336,7 @@
         <v>83</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3825,395 +3344,263 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
       <c r="C35">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B36">
         <v>5</v>
       </c>
       <c r="C36">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B37">
         <v>6</v>
       </c>
       <c r="C37">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>82</v>
+      <c r="A42" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45">
         <v>2</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
       <c r="C45">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46">
-        <v>6</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47">
-        <v>7</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48">
-        <v>8</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49">
-        <v>9</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>265</v>
-      </c>
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
+      <c r="A56" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57">
-        <v>2</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>200</v>
-      </c>
+      <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59">
-        <v>200</v>
-      </c>
+      <c r="A59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60">
-        <v>3</v>
-      </c>
-      <c r="C60">
-        <v>200</v>
-      </c>
+      <c r="A60" s="3"/>
     </row>
     <row r="71" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M71" s="3"/>
@@ -4229,7 +3616,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4324,7 +3711,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B10" sqref="B4:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,8 +4253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4999,10 +4386,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A3:A11"/>
+  <dimension ref="A3:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:H20"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5032,26 +4419,21 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5267,10 +4649,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC2358-B737-4B12-BCF2-983233884487}">
-  <dimension ref="A3:B20"/>
+  <dimension ref="A3:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,14 +4797,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5432,8 +4806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A3:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5528,9 +4902,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5562,8 +4934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,7 +5050,7 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -5700,7 +5072,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -5711,7 +5083,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -5719,35 +5091,35 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5755,10 +5127,10 @@
         <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5766,10 +5138,10 @@
         <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5777,81 +5149,81 @@
         <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -5862,7 +5234,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -5873,10 +5245,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -5884,7 +5256,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -5895,10 +5267,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -5906,245 +5278,101 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>66</v>
+      <c r="A34" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>66</v>
+      <c r="A35" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>66</v>
+      <c r="A36" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>82</v>
+      <c r="A39" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="C39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
+      <c r="A48" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6157,8 +5385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A3:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6305,7 +5533,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -6316,7 +5544,7 @@
         <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -6327,7 +5555,7 @@
         <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -6338,7 +5566,7 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -6346,35 +5574,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6382,10 +5610,10 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6393,10 +5621,10 @@
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6404,76 +5632,76 @@
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="C30">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6481,10 +5709,10 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6495,7 +5723,7 @@
         <v>29</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6503,10 +5731,10 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6517,7 +5745,7 @@
         <v>29</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6525,10 +5753,10 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6539,147 +5767,147 @@
         <v>29</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
         <v>29</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6687,10 +5915,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -6698,271 +5926,53 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>82</v>
+      <c r="A53" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C62">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B72" t="s">
-        <v>34</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" t="s">
-        <v>90</v>
-      </c>
-      <c r="C74">
-        <v>3</v>
-      </c>
       <c r="F74" s="3"/>
     </row>
   </sheetData>
@@ -6972,10 +5982,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
-  <dimension ref="A3:A12"/>
+  <dimension ref="A3:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7016,21 +6026,6 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -7127,10 +6122,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
-  <dimension ref="A3:B11"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7172,23 +6167,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7196,17 +6191,9 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11">
         <v>0</v>
       </c>
     </row>
@@ -7217,10 +6204,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
-  <dimension ref="A3:B20"/>
+  <dimension ref="A3:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7361,14 +6348,6 @@
         <v>88</v>
       </c>
       <c r="B19">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20">
         <v>100000</v>
       </c>
     </row>
@@ -7527,7 +6506,7 @@
   <dimension ref="A3:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7555,7 +6534,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7726,15 +6705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -7745,7 +6715,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -7946,15 +6916,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -7971,7 +6942,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7988,4 +6959,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Klar for kjøringer med parse
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B583B9-8B57-41EA-8B0C-E0361A2C9B4C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -6442,8 +6442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB31CFC9-E7A6-4B4A-99A3-E708E722ECEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6505,8 +6505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y33" sqref="Y33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
oppdatert CCS efficiencies til likt som genesys (10 % ned)
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B583B9-8B57-41EA-8B0C-E0361A2C9B4C}"/>
+  <xr:revisionPtr revIDLastSave="452" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44FE1B8F-529B-40A1-B5ED-33946B09E80C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -1988,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2276,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="D23">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,7 +2332,7 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>0.93</v>
+        <v>0.83700000000000008</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="D41">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>4</v>
       </c>
       <c r="D43">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>4</v>
       </c>
       <c r="D44">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2627,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="D45">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2641,7 +2641,7 @@
         <v>5</v>
       </c>
       <c r="D46">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="H46" s="3"/>
     </row>
@@ -2656,7 +2656,7 @@
         <v>6</v>
       </c>
       <c r="D47">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="H47" s="3"/>
     </row>
@@ -2671,7 +2671,7 @@
         <v>6</v>
       </c>
       <c r="D48">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="H48" s="3"/>
     </row>
@@ -2776,7 +2776,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,7 +3711,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B4:B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,7 +3806,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B11" sqref="B11:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6442,8 +6442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB31CFC9-E7A6-4B4A-99A3-E708E722ECEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6705,6 +6705,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6715,7 +6724,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6916,16 +6925,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6942,7 +6950,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6959,12 +6967,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fikset load shift cost til 1
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Kjøre kode/05.05/Simple_extended-4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Simple_extended-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="452" documentId="13_ncr:1_{0856EC59-8951-4174-A775-741DBBFD32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44FE1B8F-529B-40A1-B5ED-33946B09E80C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA613CF6-88B2-4EDF-81E8-2B9B132EBCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="26" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -1988,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -6124,8 +6124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3B805B-55A4-438A-A6DD-569B37D83033}">
   <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6146,7 +6146,7 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6154,7 +6154,7 @@
         <v>34</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6162,7 +6162,7 @@
         <v>35</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6178,7 +6178,7 @@
         <v>31</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Klar for alu case
</commit_message>
<xml_diff>
--- a/Test_data_simple_extended_reduced.xlsx
+++ b/Test_data_simple_extended_reduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\v6\Simple_extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17255961-6C73-482E-918C-DB50B39E9364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B803AF-8917-41A3-B924-AC07A2E61B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="19" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -2776,7 +2776,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,7 +2817,7 @@
         <v>64</v>
       </c>
       <c r="B5">
-        <v>1121.9639999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>76</v>
       </c>
       <c r="B6">
-        <v>32.186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,7 +3674,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3710,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,7 +3769,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3806,7 +3806,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B4" sqref="B4:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,7 +3838,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3854,7 +3854,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3862,7 +3862,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3870,7 +3870,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3878,7 +3878,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3902,7 +3902,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3910,7 +3910,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +3926,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3934,7 +3934,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3942,7 +3942,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3950,7 +3950,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3958,7 +3958,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,7 +3966,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3974,7 +3974,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3998,7 +3998,7 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4014,7 +4014,7 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -4035,7 +4035,7 @@
   <dimension ref="A3:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B4" sqref="B4:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4065,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4081,7 +4081,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4121,7 +4121,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4129,7 +4129,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4137,7 +4137,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4145,7 +4145,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4153,7 +4153,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4169,7 +4169,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4177,7 +4177,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4193,7 +4193,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -4217,7 +4217,7 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4233,7 +4233,7 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4241,7 +4241,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -4388,8 +4388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A3:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6705,6 +6705,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6905,7 +6916,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6914,18 +6925,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6944,27 +6961,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>